<commit_message>
moved images and added new runs for CMC and chitin CO2
</commit_message>
<xml_diff>
--- a/1-data/dry_ash weight_carbstore.xlsx
+++ b/1-data/dry_ash weight_carbstore.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garc286/RStudio/mibro_SFA/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garc286/RStudio/sfa_msc2_conditions/1-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0207C3EA-261D-8549-95B8-9ABCEB2DE79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCE29D3-6542-9947-8D3D-75AD032F862B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15560" xr2:uid="{74420E93-5BCF-9F48-B545-ED23A1E53012}"/>
   </bookViews>
@@ -337,7 +337,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -625,7 +625,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -636,8 +636,8 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F58" sqref="F58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>